<commit_message>
Version as of January 23rd, before update
</commit_message>
<xml_diff>
--- a/Data.xlsx
+++ b/Data.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12360" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12360" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Generators" sheetId="5" r:id="rId1"/>
@@ -1073,6 +1073,7 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1100,7 +1101,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1435,14 +1435,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="33" t="s">
+      <c r="A1" s="34" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="34"/>
-      <c r="C1" s="34"/>
-      <c r="D1" s="34"/>
-      <c r="E1" s="34"/>
-      <c r="F1" s="35"/>
+      <c r="B1" s="35"/>
+      <c r="C1" s="35"/>
+      <c r="D1" s="35"/>
+      <c r="E1" s="35"/>
+      <c r="F1" s="36"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="11" t="s">
@@ -1589,14 +1589,14 @@
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="33" t="s">
+      <c r="A10" s="34" t="s">
         <v>1</v>
       </c>
-      <c r="B10" s="34"/>
-      <c r="C10" s="34"/>
-      <c r="D10" s="34"/>
-      <c r="E10" s="34"/>
-      <c r="F10" s="35"/>
+      <c r="B10" s="35"/>
+      <c r="C10" s="35"/>
+      <c r="D10" s="35"/>
+      <c r="E10" s="35"/>
+      <c r="F10" s="36"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="11" t="s">
@@ -1746,14 +1746,14 @@
       <c r="E18" s="5"/>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" s="33" t="s">
+      <c r="A19" s="34" t="s">
         <v>2</v>
       </c>
-      <c r="B19" s="34"/>
-      <c r="C19" s="34"/>
-      <c r="D19" s="34"/>
-      <c r="E19" s="34"/>
-      <c r="F19" s="35"/>
+      <c r="B19" s="35"/>
+      <c r="C19" s="35"/>
+      <c r="D19" s="35"/>
+      <c r="E19" s="35"/>
+      <c r="F19" s="36"/>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="11" t="s">
@@ -1903,14 +1903,14 @@
       <c r="E27" s="5"/>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A28" s="33" t="s">
+      <c r="A28" s="34" t="s">
         <v>3</v>
       </c>
-      <c r="B28" s="34"/>
-      <c r="C28" s="34"/>
-      <c r="D28" s="34"/>
-      <c r="E28" s="34"/>
-      <c r="F28" s="35"/>
+      <c r="B28" s="35"/>
+      <c r="C28" s="35"/>
+      <c r="D28" s="35"/>
+      <c r="E28" s="35"/>
+      <c r="F28" s="36"/>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" s="11" t="s">
@@ -2060,14 +2060,14 @@
       <c r="E36" s="5"/>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A37" s="33" t="s">
+      <c r="A37" s="34" t="s">
         <v>4</v>
       </c>
-      <c r="B37" s="34"/>
-      <c r="C37" s="34"/>
-      <c r="D37" s="34"/>
-      <c r="E37" s="34"/>
-      <c r="F37" s="35"/>
+      <c r="B37" s="35"/>
+      <c r="C37" s="35"/>
+      <c r="D37" s="35"/>
+      <c r="E37" s="35"/>
+      <c r="F37" s="36"/>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" s="11" t="s">
@@ -2415,7 +2415,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="P4" sqref="P4"/>
     </sheetView>
   </sheetViews>
@@ -2432,31 +2432,31 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A1" s="36" t="s">
+      <c r="A1" s="37" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="37"/>
-      <c r="C1" s="38"/>
-      <c r="D1" s="36" t="s">
+      <c r="B1" s="38"/>
+      <c r="C1" s="39"/>
+      <c r="D1" s="37" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="37"/>
-      <c r="F1" s="38"/>
-      <c r="G1" s="36" t="s">
+      <c r="E1" s="38"/>
+      <c r="F1" s="39"/>
+      <c r="G1" s="37" t="s">
         <v>2</v>
       </c>
-      <c r="H1" s="37"/>
-      <c r="I1" s="38"/>
-      <c r="J1" s="36" t="s">
+      <c r="H1" s="38"/>
+      <c r="I1" s="39"/>
+      <c r="J1" s="37" t="s">
         <v>3</v>
       </c>
-      <c r="K1" s="37"/>
-      <c r="L1" s="38"/>
-      <c r="M1" s="39" t="s">
+      <c r="K1" s="38"/>
+      <c r="L1" s="39"/>
+      <c r="M1" s="40" t="s">
         <v>4</v>
       </c>
-      <c r="N1" s="40"/>
-      <c r="O1" s="40"/>
+      <c r="N1" s="41"/>
+      <c r="O1" s="41"/>
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A2" s="9" t="s">
@@ -4454,7 +4454,7 @@
       </c>
     </row>
     <row r="34" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="C34" s="42"/>
+      <c r="C34" s="33"/>
       <c r="F34" s="18"/>
     </row>
   </sheetData>
@@ -4497,31 +4497,31 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A1" s="33" t="s">
+      <c r="A1" s="34" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="34"/>
-      <c r="C1" s="35"/>
-      <c r="E1" s="33" t="s">
+      <c r="B1" s="35"/>
+      <c r="C1" s="36"/>
+      <c r="E1" s="34" t="s">
         <v>1</v>
       </c>
-      <c r="F1" s="34"/>
-      <c r="G1" s="35"/>
-      <c r="I1" s="33" t="s">
+      <c r="F1" s="35"/>
+      <c r="G1" s="36"/>
+      <c r="I1" s="34" t="s">
         <v>2</v>
       </c>
-      <c r="J1" s="34"/>
-      <c r="K1" s="35"/>
-      <c r="M1" s="33" t="s">
+      <c r="J1" s="35"/>
+      <c r="K1" s="36"/>
+      <c r="M1" s="34" t="s">
         <v>3</v>
       </c>
-      <c r="N1" s="34"/>
-      <c r="O1" s="35"/>
-      <c r="Q1" s="33" t="s">
+      <c r="N1" s="35"/>
+      <c r="O1" s="36"/>
+      <c r="Q1" s="34" t="s">
         <v>4</v>
       </c>
-      <c r="R1" s="34"/>
-      <c r="S1" s="35"/>
+      <c r="R1" s="35"/>
+      <c r="S1" s="36"/>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A2" s="11" t="s">
@@ -5577,8 +5577,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="U4" sqref="U4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5596,31 +5596,31 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A1" s="33" t="s">
+      <c r="A1" s="34" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="34"/>
-      <c r="C1" s="35"/>
-      <c r="E1" s="33" t="s">
+      <c r="B1" s="35"/>
+      <c r="C1" s="36"/>
+      <c r="E1" s="34" t="s">
         <v>1</v>
       </c>
-      <c r="F1" s="34"/>
-      <c r="G1" s="35"/>
-      <c r="I1" s="33" t="s">
+      <c r="F1" s="35"/>
+      <c r="G1" s="36"/>
+      <c r="I1" s="34" t="s">
         <v>2</v>
       </c>
-      <c r="J1" s="34"/>
-      <c r="K1" s="35"/>
-      <c r="M1" s="33" t="s">
+      <c r="J1" s="35"/>
+      <c r="K1" s="36"/>
+      <c r="M1" s="34" t="s">
         <v>3</v>
       </c>
-      <c r="N1" s="34"/>
-      <c r="O1" s="35"/>
-      <c r="Q1" s="33" t="s">
+      <c r="N1" s="35"/>
+      <c r="O1" s="36"/>
+      <c r="Q1" s="34" t="s">
         <v>4</v>
       </c>
-      <c r="R1" s="34"/>
-      <c r="S1" s="35"/>
+      <c r="R1" s="35"/>
+      <c r="S1" s="36"/>
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A2" s="11" t="s">
@@ -5729,8 +5729,8 @@
       <c r="B4" s="14">
         <v>1E+30</v>
       </c>
-      <c r="C4" s="21">
-        <v>1</v>
+      <c r="C4" s="16">
+        <v>3</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>154</v>
@@ -6528,7 +6528,7 @@
       <c r="B22" s="29"/>
       <c r="C22" s="30">
         <f>SUM(C3:C20)</f>
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="D22" s="32"/>
       <c r="E22" s="28" t="s">
@@ -6568,7 +6568,7 @@
       </c>
       <c r="T22" s="31">
         <f>SUM(C22,G22,K22,O22,S22)</f>
-        <v>315</v>
+        <v>317</v>
       </c>
     </row>
   </sheetData>
@@ -6598,14 +6598,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="41" t="s">
+      <c r="A1" s="42" t="s">
         <v>187</v>
       </c>
-      <c r="B1" s="41"/>
-      <c r="D1" s="41" t="s">
+      <c r="B1" s="42"/>
+      <c r="D1" s="42" t="s">
         <v>257</v>
       </c>
-      <c r="E1" s="41"/>
+      <c r="E1" s="42"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
@@ -6898,12 +6898,12 @@
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A34" s="41" t="s">
+      <c r="A34" s="42" t="s">
         <v>255</v>
       </c>
-      <c r="B34" s="41"/>
-      <c r="C34" s="41"/>
-      <c r="D34" s="41"/>
+      <c r="B34" s="42"/>
+      <c r="C34" s="42"/>
+      <c r="D34" s="42"/>
     </row>
   </sheetData>
   <mergeCells count="3">

</xml_diff>